<commit_message>
Invoice Generating is done
</commit_message>
<xml_diff>
--- a/MajoliFE/Templates/invoice_majoli_template.xlsx
+++ b/MajoliFE/Templates/invoice_majoli_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nenad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJEKTI\MajoliFE\MajoliFE\MajoliFE\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4277949F-0C2D-4BDF-B7B9-F2A5319A122F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E5C434-A522-4D11-9CD8-EDF0FD33236F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1320" windowWidth="29040" windowHeight="15840" xr2:uid="{E3E6C6C7-1AC3-4530-8AF5-D5FEB8985BB8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <r>
       <rPr>
@@ -403,16 +403,6 @@
         <family val="2"/>
       </rPr>
       <t>Mesto izdavanja</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Po dokumentu</t>
     </r>
   </si>
   <si>
@@ -1291,14 +1281,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1308,118 +1347,115 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1428,8 +1464,212 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1457,6 +1697,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
@@ -1464,281 +1707,19 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1859,10 +1840,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2162,10 +2139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B377A1C2-DC0D-4508-B288-E47FB30E63FD}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,752 +2154,732 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="94"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="94"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="94"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+    </row>
+    <row r="5" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="94"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+    </row>
+    <row r="6" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="96" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="97"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="98"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="99"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="101"/>
+    </row>
+    <row r="8" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="102"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="104"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="81"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="86">
+        <v>1001</v>
+      </c>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="152"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="152"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="152"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-    </row>
-    <row r="5" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="152"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-    </row>
-    <row r="6" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="149" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="91"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87"/>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="92"/>
-    </row>
-    <row r="8" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="150"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="94"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="147" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="58">
-        <v>1001</v>
-      </c>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="111" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="111"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="112" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="112"/>
-      <c r="N9" s="80"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="106" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="106"/>
+      <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="148"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="96" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="67"/>
     </row>
     <row r="11" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="146" t="s">
+      <c r="A11" s="74" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="75"/>
       <c r="C11" s="76"/>
       <c r="D11" s="77" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="78"/>
       <c r="F11" s="78"/>
       <c r="G11" s="79"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="65"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="70"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="146" t="s">
+      <c r="A12" s="74" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="75"/>
       <c r="C12" s="76"/>
       <c r="D12" s="77" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="78"/>
       <c r="F12" s="78"/>
       <c r="G12" s="79"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="65"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="70"/>
     </row>
     <row r="13" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="146" t="s">
+      <c r="A13" s="74" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="75"/>
       <c r="C13" s="76"/>
       <c r="D13" s="77" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="78"/>
       <c r="F13" s="78"/>
       <c r="G13" s="79"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="68"/>
-    </row>
-    <row r="14" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="146" t="s">
+      <c r="H13" s="71"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="73"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="75"/>
       <c r="C14" s="76"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="85"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="146" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="97" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="99">
+      <c r="D14" s="107" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="15">
         <v>60</v>
       </c>
-      <c r="H15" s="83"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="85"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="78"/>
+      <c r="N14" s="79"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="127"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="128"/>
+      <c r="L15" s="128"/>
+      <c r="M15" s="128"/>
+      <c r="N15" s="129"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="145"/>
-      <c r="B16" s="130"/>
-      <c r="C16" s="130"/>
-      <c r="D16" s="130"/>
-      <c r="E16" s="130"/>
-      <c r="F16" s="130"/>
-      <c r="G16" s="130"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="130"/>
-      <c r="J16" s="130"/>
-      <c r="K16" s="130"/>
-      <c r="L16" s="130"/>
-      <c r="M16" s="130"/>
-      <c r="N16" s="134"/>
+      <c r="A16" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="47"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="49" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="143" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="50"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1005251</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="52"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="5">
+        <v>4</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="6">
         <v>0</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" s="10"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="144"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="N18" s="23"/>
+      <c r="J18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="L18" s="7">
+        <v>20</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="142">
-        <v>1</v>
-      </c>
-      <c r="B19" s="24">
-        <v>1005251</v>
-      </c>
-      <c r="C19" s="95" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="28">
-        <v>4</v>
-      </c>
-      <c r="H19" s="109" t="s">
+      <c r="A19" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="29">
+      <c r="M19" s="37"/>
+      <c r="N19" s="38"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="57"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="58">
         <v>0</v>
       </c>
-      <c r="J19" s="110" t="s">
+      <c r="M20" s="37"/>
+      <c r="N20" s="38"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="60"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="125" t="s">
+      <c r="E21" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="L19" s="30">
-        <v>20</v>
-      </c>
-      <c r="M19" s="125" t="s">
+      <c r="F21" s="63"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="M21" s="37"/>
+      <c r="N21" s="38"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="145"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="M22" s="37"/>
+      <c r="N22" s="38"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="145"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="146"/>
+      <c r="H23" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="M23" s="37"/>
+      <c r="N23" s="38"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="145"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="146"/>
+      <c r="H24" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="N19" s="125" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="126" t="s">
-        <v>49</v>
-      </c>
-      <c r="M20" s="101"/>
-      <c r="N20" s="102"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="140" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="100">
-        <v>0</v>
-      </c>
-      <c r="M21" s="101"/>
-      <c r="N21" s="102"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="139" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="128" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="129" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="105"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="126" t="s">
-        <v>49</v>
-      </c>
-      <c r="M22" s="101"/>
-      <c r="N22" s="102"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="86"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="126" t="s">
-        <v>49</v>
-      </c>
-      <c r="M23" s="101"/>
-      <c r="N23" s="102"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="86"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="126" t="s">
-        <v>50</v>
-      </c>
-      <c r="M24" s="101"/>
-      <c r="N24" s="102"/>
+      <c r="M24" s="131"/>
+      <c r="N24" s="132"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="86"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="127" t="s">
-        <v>51</v>
-      </c>
-      <c r="M25" s="103"/>
-      <c r="N25" s="104"/>
+      <c r="A25" s="145"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="146"/>
+      <c r="H25" s="133"/>
+      <c r="I25" s="134"/>
+      <c r="J25" s="134"/>
+      <c r="K25" s="134"/>
+      <c r="L25" s="134"/>
+      <c r="M25" s="134"/>
+      <c r="N25" s="135"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="86"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="49"/>
+      <c r="A26" s="145"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="136" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="137"/>
+      <c r="J26" s="137"/>
+      <c r="K26" s="137"/>
+      <c r="L26" s="137"/>
+      <c r="M26" s="137"/>
+      <c r="N26" s="138"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="86"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="52"/>
+      <c r="A27" s="145"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="146"/>
+      <c r="H27" s="139" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="140"/>
+      <c r="J27" s="140"/>
+      <c r="K27" s="141"/>
+      <c r="L27" s="139" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" s="140"/>
+      <c r="N27" s="141"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="86"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="M28" s="54"/>
-      <c r="N28" s="55"/>
+      <c r="A28" s="147"/>
+      <c r="B28" s="148"/>
+      <c r="C28" s="148"/>
+      <c r="D28" s="148"/>
+      <c r="E28" s="148"/>
+      <c r="F28" s="148"/>
+      <c r="G28" s="149"/>
+      <c r="H28" s="139" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="140"/>
+      <c r="J28" s="140"/>
+      <c r="K28" s="141"/>
+      <c r="L28" s="142" t="s">
+        <v>43</v>
+      </c>
+      <c r="M28" s="143"/>
+      <c r="N28" s="144"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="138"/>
-      <c r="B29" s="106"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="108" t="s">
+      <c r="A29" s="115"/>
+      <c r="B29" s="116"/>
+      <c r="C29" s="116"/>
+      <c r="D29" s="116"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="116"/>
+      <c r="G29" s="116"/>
+      <c r="H29" s="116"/>
+      <c r="I29" s="116"/>
+      <c r="J29" s="116"/>
+      <c r="K29" s="116"/>
+      <c r="L29" s="116"/>
+      <c r="M29" s="116"/>
+      <c r="N29" s="117"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="109" t="s">
         <v>44</v>
       </c>
-      <c r="M29" s="56"/>
-      <c r="N29" s="57"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="137"/>
-      <c r="B30" s="119"/>
-      <c r="C30" s="119"/>
-      <c r="D30" s="119"/>
-      <c r="E30" s="119"/>
-      <c r="F30" s="119"/>
-      <c r="G30" s="119"/>
-      <c r="H30" s="119"/>
-      <c r="I30" s="119"/>
-      <c r="J30" s="119"/>
-      <c r="K30" s="119"/>
-      <c r="L30" s="119"/>
-      <c r="M30" s="119"/>
-      <c r="N30" s="133"/>
+      <c r="B30" s="110"/>
+      <c r="C30" s="110"/>
+      <c r="D30" s="110"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="110"/>
+      <c r="G30" s="110"/>
+      <c r="H30" s="110"/>
+      <c r="I30" s="110"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="110"/>
+      <c r="L30" s="110"/>
+      <c r="M30" s="110"/>
+      <c r="N30" s="111"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="113" t="s">
+      <c r="A31" s="112"/>
+      <c r="B31" s="113"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="113"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="113"/>
+      <c r="I31" s="113"/>
+      <c r="J31" s="113"/>
+      <c r="K31" s="113"/>
+      <c r="L31" s="113"/>
+      <c r="M31" s="113"/>
+      <c r="N31" s="114"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="124"/>
+      <c r="B32" s="125"/>
+      <c r="C32" s="125"/>
+      <c r="D32" s="125"/>
+      <c r="E32" s="125"/>
+      <c r="F32" s="125"/>
+      <c r="G32" s="125"/>
+      <c r="H32" s="125"/>
+      <c r="I32" s="125"/>
+      <c r="J32" s="125"/>
+      <c r="K32" s="125"/>
+      <c r="L32" s="125"/>
+      <c r="M32" s="125"/>
+      <c r="N32" s="126"/>
+    </row>
+    <row r="33" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="114"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="114"/>
-      <c r="H31" s="114"/>
-      <c r="I31" s="114"/>
-      <c r="J31" s="114"/>
-      <c r="K31" s="114"/>
-      <c r="L31" s="114"/>
-      <c r="M31" s="114"/>
-      <c r="N31" s="115"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="116"/>
-      <c r="B32" s="117"/>
-      <c r="C32" s="117"/>
-      <c r="D32" s="117"/>
-      <c r="E32" s="117"/>
-      <c r="F32" s="117"/>
-      <c r="G32" s="117"/>
-      <c r="H32" s="117"/>
-      <c r="I32" s="117"/>
-      <c r="J32" s="117"/>
-      <c r="K32" s="117"/>
-      <c r="L32" s="117"/>
-      <c r="M32" s="117"/>
-      <c r="N32" s="118"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="136"/>
-      <c r="B33" s="120"/>
-      <c r="C33" s="120"/>
-      <c r="D33" s="120"/>
-      <c r="E33" s="120"/>
-      <c r="F33" s="120"/>
-      <c r="G33" s="120"/>
-      <c r="H33" s="120"/>
-      <c r="I33" s="120"/>
-      <c r="J33" s="120"/>
-      <c r="K33" s="120"/>
-      <c r="L33" s="120"/>
-      <c r="M33" s="120"/>
-      <c r="N33" s="132"/>
-    </row>
-    <row r="34" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="135" t="s">
+      <c r="B33" s="119"/>
+      <c r="C33" s="119"/>
+      <c r="D33" s="119"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="123"/>
+      <c r="G33" s="123"/>
+      <c r="H33" s="123"/>
+      <c r="I33" s="123"/>
+      <c r="J33" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="122"/>
-      <c r="C34" s="122"/>
-      <c r="D34" s="122"/>
-      <c r="E34" s="123"/>
-      <c r="F34" s="123"/>
-      <c r="G34" s="123"/>
-      <c r="H34" s="123"/>
-      <c r="I34" s="123"/>
-      <c r="J34" s="124" t="s">
-        <v>47</v>
-      </c>
-      <c r="K34" s="121"/>
-      <c r="L34" s="121"/>
-      <c r="M34" s="121"/>
-      <c r="N34" s="131"/>
+      <c r="K33" s="121"/>
+      <c r="L33" s="121"/>
+      <c r="M33" s="121"/>
+      <c r="N33" s="122"/>
     </row>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="A31:N32"/>
-    <mergeCell ref="A30:N30"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="A33:N33"/>
-    <mergeCell ref="A16:N16"/>
+  <mergeCells count="61">
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="A22:G28"/>
+    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="H25:N25"/>
+    <mergeCell ref="H26:N26"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="A30:N31"/>
+    <mergeCell ref="A29:N29"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="A32:N32"/>
     <mergeCell ref="A1:J5"/>
     <mergeCell ref="K1:N5"/>
     <mergeCell ref="A6:N8"/>
     <mergeCell ref="H9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="H10:N13"/>
-    <mergeCell ref="H14:N14"/>
-    <mergeCell ref="H15:N15"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
     <mergeCell ref="D11:G11"/>
     <mergeCell ref="D12:G12"/>
     <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
     <mergeCell ref="A9:C10"/>
     <mergeCell ref="D9:G10"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="H26:N26"/>
-    <mergeCell ref="H27:N27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="A23:G29"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="L22:N22"/>
     <mergeCell ref="H23:K23"/>
     <mergeCell ref="L23:N23"/>
     <mergeCell ref="H24:K24"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="H21:K21"/>
     <mergeCell ref="L21:N21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Production improvements, added Vendors, added vendorInvoices, added statistics
</commit_message>
<xml_diff>
--- a/MajoliFE/Templates/invoice_majoli_template.xlsx
+++ b/MajoliFE/Templates/invoice_majoli_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJEKTI\MajoliFE\MajoliFE\MajoliFE\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6DF15A-C12B-43AB-A402-526EA58866CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA926FD-0BA2-4FA7-8ECF-C53F793D1EB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1320" windowWidth="29040" windowHeight="15840" xr2:uid="{E3E6C6C7-1AC3-4530-8AF5-D5FEB8985BB8}"/>
   </bookViews>
@@ -453,6 +453,10 @@
     <t>Nema napomene</t>
   </si>
   <si>
+    <t xml:space="preserve">Za Prodavca                                             
+</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -461,8 +465,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Za kupca                                             
-</t>
+      <t xml:space="preserve">Za kupca                                              </t>
     </r>
     <r>
       <rPr>
@@ -471,13 +474,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">
-Broj L.K.                                               </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Za Prodavca                                             
-</t>
+      <t>Broj L.K.                                    </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1226,7 +1224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -1343,6 +1341,45 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1520,45 +1557,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1607,12 +1605,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1665,6 +1657,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1745,7 +1740,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>220538</xdr:colOff>
+      <xdr:colOff>391988</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>131151</xdr:rowOff>
     </xdr:to>
@@ -2084,259 +2079,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B377A1C2-DC0D-4508-B288-E47FB30E63FD}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33:N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
+      <c r="A3" s="73"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
+      <c r="A4" s="73"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
     </row>
     <row r="5" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
     </row>
     <row r="6" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="63"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="64"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="77"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="67"/>
+      <c r="A7" s="78"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="80"/>
     </row>
     <row r="8" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="68"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="70"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="83"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="72" t="s">
+      <c r="B9" s="101"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="72"/>
+      <c r="M9" s="85"/>
       <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="90"/>
-      <c r="B10" s="91"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="75"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="88"/>
     </row>
     <row r="11" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="76"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="89"/>
       <c r="I11" s="23"/>
       <c r="J11" s="23"/>
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23"/>
-      <c r="N11" s="77"/>
+      <c r="N11" s="90"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="82"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="76"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="99"/>
+      <c r="H12" s="89"/>
       <c r="I12" s="23"/>
       <c r="J12" s="23"/>
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
-      <c r="N12" s="77"/>
+      <c r="N12" s="90"/>
     </row>
     <row r="13" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="80"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="92"/>
+      <c r="M13" s="92"/>
+      <c r="N13" s="93"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="82"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="86"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="99"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
@@ -2355,30 +2362,30 @@
       <c r="N15" s="30"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="138" t="s">
+      <c r="A16" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="140" t="s">
+      <c r="B16" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="143"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="148" t="s">
+      <c r="D16" s="141"/>
+      <c r="E16" s="142"/>
+      <c r="F16" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="148" t="s">
+      <c r="G16" s="146" t="s">
         <v>4</v>
       </c>
       <c r="H16" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="110" t="s">
+      <c r="I16" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="112" t="s">
+      <c r="J16" s="51" t="s">
         <v>7</v>
       </c>
       <c r="K16" s="114" t="s">
@@ -2391,16 +2398,16 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="139"/>
-      <c r="B17" s="141"/>
-      <c r="C17" s="145"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="147"/>
-      <c r="F17" s="149"/>
-      <c r="G17" s="149"/>
+      <c r="A17" s="137"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="147"/>
+      <c r="G17" s="147"/>
       <c r="H17" s="123"/>
-      <c r="I17" s="111"/>
-      <c r="J17" s="113"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="52"/>
       <c r="K17" s="1" t="s">
         <v>10</v>
       </c>
@@ -2432,21 +2439,21 @@
       <c r="A19" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="108"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="109"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="48"/>
       <c r="G19" s="125"/>
-      <c r="H19" s="101" t="s">
+      <c r="H19" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="102"/>
-      <c r="J19" s="102"/>
-      <c r="K19" s="103"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="105"/>
-      <c r="N19" s="106"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="45"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="127" t="s">
@@ -2457,40 +2464,40 @@
       <c r="D20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="130" t="s">
+      <c r="E20" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="131"/>
+      <c r="F20" s="129"/>
       <c r="G20" s="126"/>
-      <c r="H20" s="101" t="s">
+      <c r="H20" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="102"/>
-      <c r="J20" s="102"/>
-      <c r="K20" s="103"/>
-      <c r="L20" s="132"/>
-      <c r="M20" s="105"/>
-      <c r="N20" s="106"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="130"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="45"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="133" t="s">
+      <c r="A21" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="134"/>
-      <c r="C21" s="135"/>
+      <c r="B21" s="132"/>
+      <c r="C21" s="133"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="137"/>
+      <c r="E21" s="134"/>
+      <c r="F21" s="135"/>
       <c r="G21" s="126"/>
-      <c r="H21" s="101" t="s">
+      <c r="H21" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="102"/>
-      <c r="J21" s="102"/>
-      <c r="K21" s="103"/>
-      <c r="L21" s="104"/>
-      <c r="M21" s="105"/>
-      <c r="N21" s="106"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="45"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
@@ -2500,15 +2507,15 @@
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
       <c r="G22" s="24"/>
-      <c r="H22" s="101" t="s">
+      <c r="H22" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="103"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="106"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="45"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
@@ -2518,15 +2525,15 @@
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
       <c r="G23" s="24"/>
-      <c r="H23" s="101" t="s">
+      <c r="H23" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="102"/>
-      <c r="J23" s="102"/>
-      <c r="K23" s="103"/>
-      <c r="L23" s="104"/>
-      <c r="M23" s="105"/>
-      <c r="N23" s="106"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="45"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
@@ -2536,12 +2543,12 @@
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
       <c r="G24" s="24"/>
-      <c r="H24" s="107" t="s">
+      <c r="H24" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="108"/>
-      <c r="J24" s="108"/>
-      <c r="K24" s="109"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="48"/>
       <c r="L24" s="31"/>
       <c r="M24" s="32"/>
       <c r="N24" s="33"/>
@@ -2617,90 +2624,90 @@
       <c r="N28" s="21"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="48"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="61"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="42"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="55"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="45"/>
+      <c r="A31" s="56"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="58"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="57"/>
+      <c r="A32" s="68"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="70"/>
     </row>
     <row r="33" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="53"/>
+      <c r="K33" s="65"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="61">
@@ -2767,7 +2774,7 @@
     <mergeCell ref="J16:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="83" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added reports for all invoices and all vendor invoices with statistics, added statistics to vendor invoices page
</commit_message>
<xml_diff>
--- a/MajoliFE/Templates/invoice_majoli_template.xlsx
+++ b/MajoliFE/Templates/invoice_majoli_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJEKTI\MajoliFE\MajoliFE\MajoliFE\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA926FD-0BA2-4FA7-8ECF-C53F793D1EB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB74B628-98D0-4B5A-9CDD-E496EACDCAA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1320" windowWidth="29040" windowHeight="15840" xr2:uid="{E3E6C6C7-1AC3-4530-8AF5-D5FEB8985BB8}"/>
   </bookViews>
@@ -399,57 +399,6 @@
     <t>Broj paketa:</t>
   </si>
   <si>
-    <t>Račun - OTPREMNICA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Majoli d.o.o. za trgovinu na veliko
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Sedište: 1. Maja 12 18330 Babušnica</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="6"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>PIB: 109768;
-Mat.br.: 21239372; 
-EPPDV: 01.11.2016.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="6"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>Nema napomene</t>
   </si>
   <si>
@@ -475,6 +424,33 @@
         <family val="2"/>
       </rPr>
       <t>Broj L.K.                                    </t>
+    </r>
+  </si>
+  <si>
+    <t>RAČUN - OTPREMNICA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Majoli d.o.o. za trgovinu na veliko
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sedište: 1. Maja 12 18330 Babušnica
+PIB: 109768;
+Mat.br.: 21239372; 
+EPPDV: 01.11.2016.
+</t>
     </r>
   </si>
 </sst>
@@ -485,7 +461,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0."/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,11 +546,6 @@
     <font>
       <sz val="6"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -660,7 +631,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -927,15 +898,6 @@
         <color rgb="FF7F7F7F"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -997,15 +959,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1054,167 +1007,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
@@ -1224,7 +1023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -1250,7 +1049,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -1263,55 +1061,247 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1320,52 +1310,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1380,287 +1337,54 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2084,8 +1808,8 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33:N33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,25 +1830,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
+      <c r="A1" s="107" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="110"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
+      <c r="A2" s="111"/>
       <c r="B2" s="72"/>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
@@ -2134,13 +1858,13 @@
       <c r="H2" s="72"/>
       <c r="I2" s="72"/>
       <c r="J2" s="72"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="112"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="73"/>
+      <c r="A3" s="111"/>
       <c r="B3" s="72"/>
       <c r="C3" s="72"/>
       <c r="D3" s="72"/>
@@ -2150,13 +1874,13 @@
       <c r="H3" s="72"/>
       <c r="I3" s="72"/>
       <c r="J3" s="72"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="112"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="73"/>
+      <c r="A4" s="111"/>
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="72"/>
@@ -2166,13 +1890,13 @@
       <c r="H4" s="72"/>
       <c r="I4" s="72"/>
       <c r="J4" s="72"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="112"/>
     </row>
     <row r="5" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
+      <c r="A5" s="111"/>
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="72"/>
@@ -2182,232 +1906,232 @@
       <c r="H5" s="72"/>
       <c r="I5" s="72"/>
       <c r="J5" s="72"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="112"/>
     </row>
     <row r="6" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="77"/>
+      <c r="A6" s="74" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="78"/>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="80"/>
+      <c r="A7" s="75"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
     </row>
     <row r="8" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="81"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="83"/>
+      <c r="A8" s="76"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="85" t="s">
+      <c r="B9" s="60"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="85"/>
-      <c r="N9" s="9"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="113"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="103"/>
-      <c r="B10" s="104"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="111"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="88"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
     </row>
     <row r="11" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="94" t="s">
+      <c r="A11" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="95"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="97"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="89"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="90"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="95"/>
-      <c r="C12" s="96"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="99"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="90"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
     </row>
     <row r="13" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="92"/>
-      <c r="M13" s="92"/>
-      <c r="N13" s="93"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="95"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="97"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="97"/>
-      <c r="M14" s="98"/>
-      <c r="N14" s="99"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="30"/>
+      <c r="A15" s="95"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="95"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="95"/>
+      <c r="N15" s="95"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="136" t="s">
+      <c r="A16" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="140" t="s">
+      <c r="C16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="141"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="146" t="s">
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="146" t="s">
+      <c r="G16" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="122" t="s">
+      <c r="H16" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="49" t="s">
+      <c r="I16" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="51" t="s">
+      <c r="J16" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="114" t="s">
+      <c r="K16" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L16" s="115"/>
-      <c r="M16" s="116"/>
-      <c r="N16" s="117" t="s">
+      <c r="L16" s="25"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="115" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="137"/>
-      <c r="B17" s="139"/>
-      <c r="C17" s="143"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="147"/>
-      <c r="G17" s="147"/>
-      <c r="H17" s="123"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="52"/>
+      <c r="A17" s="116"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="106"/>
       <c r="K17" s="1" t="s">
         <v>10</v>
       </c>
@@ -2417,305 +2141,340 @@
       <c r="M17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="118"/>
+      <c r="N17" s="117"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="118"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="119"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="121"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="4"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="10"/>
+      <c r="H18" s="9"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="12"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="119"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="40" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="45"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="127" t="s">
+      <c r="A20" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="128"/>
-      <c r="C20" s="129"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="148" t="s">
+      <c r="E20" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="129"/>
-      <c r="G20" s="126"/>
-      <c r="H20" s="40" t="s">
+      <c r="F20" s="42"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="130"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="45"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="131" t="s">
+      <c r="A21" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="132"/>
-      <c r="C21" s="133"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="134"/>
-      <c r="F21" s="135"/>
-      <c r="G21" s="126"/>
-      <c r="H21" s="40" t="s">
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="45"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="40" t="s">
+      <c r="A22" s="52"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="40" t="s">
+      <c r="A23" s="52"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="45"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="46" t="s">
+      <c r="A24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="33"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="96"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="97"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="36"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="99"/>
+      <c r="J25" s="99"/>
+      <c r="K25" s="99"/>
+      <c r="L25" s="99"/>
+      <c r="M25" s="99"/>
+      <c r="N25" s="99"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="37" t="s">
+      <c r="A26" s="52"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="39"/>
+      <c r="I26" s="101"/>
+      <c r="J26" s="101"/>
+      <c r="K26" s="101"/>
+      <c r="L26" s="101"/>
+      <c r="M26" s="101"/>
+      <c r="N26" s="101"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="16" t="s">
+      <c r="A27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="92"/>
+      <c r="H27" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="16" t="s">
+      <c r="I27" s="88"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="M27" s="17"/>
-      <c r="N27" s="18"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="88"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="21"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="61"/>
+      <c r="A28" s="93"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="88"/>
+      <c r="J28" s="88"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="91"/>
+      <c r="N28" s="91"/>
+    </row>
+    <row r="29" spans="1:14" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="85"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="85"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="85"/>
+      <c r="L29" s="85"/>
+      <c r="M29" s="85"/>
+      <c r="N29" s="85"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="80"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="80"/>
+      <c r="L30" s="80"/>
+      <c r="M30" s="80"/>
+      <c r="N30" s="81"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="82"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="83"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="83"/>
+      <c r="L31" s="83"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="84"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="86"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
+      <c r="N32" s="86"/>
+    </row>
+    <row r="33" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="55"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="57"/>
-      <c r="N31" s="58"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="68"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="70"/>
-    </row>
-    <row r="33" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="K33" s="65"/>
-      <c r="L33" s="65"/>
-      <c r="M33" s="65"/>
-      <c r="N33" s="66"/>
+      <c r="B33" s="121"/>
+      <c r="C33" s="121"/>
+      <c r="D33" s="121"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="122"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="122"/>
+      <c r="J33" s="123" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" s="120"/>
+      <c r="L33" s="120"/>
+      <c r="M33" s="120"/>
+      <c r="N33" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="A22:G28"/>
+    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="H25:N25"/>
+    <mergeCell ref="H26:N26"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="A30:N31"/>
+    <mergeCell ref="A29:N29"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="A32:N32"/>
+    <mergeCell ref="A1:J5"/>
+    <mergeCell ref="K1:N5"/>
+    <mergeCell ref="A6:N8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="H10:N13"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="A9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="K16:M16"/>
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="C18:E18"/>
@@ -2732,49 +2491,14 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="H21:K21"/>
     <mergeCell ref="L21:N21"/>
-    <mergeCell ref="H10:N13"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A1:J5"/>
-    <mergeCell ref="K1:N5"/>
-    <mergeCell ref="A6:N8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="A30:N31"/>
-    <mergeCell ref="A29:N29"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="A32:N32"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="A22:G28"/>
-    <mergeCell ref="A15:N15"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="H25:N25"/>
-    <mergeCell ref="H26:N26"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="83" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>